<commit_message>
[Excel Analyzer] Detect named ranges
Can be a good indication along with external links of hidden data.
</commit_message>
<xml_diff>
--- a/gems/excel_analyzer/spec/fixtures/suspect.xlsx
+++ b/gems/excel_analyzer/spec/fixtures/suspect.xlsx
@@ -5,20 +5,24 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="External Links" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Pivot Table" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Hidden Row &amp; Col" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Hidden Sheet" sheetId="4" state="hidden" r:id="rId6"/>
+    <sheet name="Ranges" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
+  <definedNames>
+    <definedName function="false" hidden="false" name="Users" vbProcedure="false">Ranges!$B$1:$B$4</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId9"/>
+    <pivotCache cacheId="1" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t xml:space="preserve">Salesperson</t>
   </si>
@@ -65,6 +69,18 @@
   </si>
   <si>
     <t xml:space="preserve">This sheet is hidden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul</t>
   </si>
 </sst>
 </file>
@@ -416,6 +432,15 @@
     <cellStyle name="Pivot Table Title" xfId="24"/>
     <cellStyle name="Pivot Table Value" xfId="25"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -668,6 +693,14 @@
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
 </pivotTableDefinition>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ID" displayName="ID" ref="A1:A4" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" name="ID"/>
+  </tableColumns>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -783,7 +816,7 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1039,12 +1072,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1073,7 +1106,7 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1086,4 +1119,63 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <tableParts>
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Excel Analyzer] Count hidden non-blank cells
We don't care about blank cells in hidden rows and columns.
</commit_message>
<xml_diff>
--- a/gems/excel_analyzer/spec/fixtures/suspect.xlsx
+++ b/gems/excel_analyzer/spec/fixtures/suspect.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="External Links" sheetId="1" state="visible" r:id="rId3"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t xml:space="preserve">Salesperson</t>
   </si>
@@ -65,7 +65,13 @@
     <t xml:space="preserve">ProductC</t>
   </si>
   <si>
-    <t xml:space="preserve">Column A or Row 1 are hidden</t>
+    <t xml:space="preserve">Column A or Row 1 are hidden with no data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column B and Row 2 are hidden with data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column C and Row 3 have zero width/height</t>
   </si>
   <si>
     <t xml:space="preserve">This sheet is hidden</t>
@@ -87,8 +93,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -325,7 +332,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1064,21 +1071,44 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:B2"/>
+  <dimension ref="B1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="3" min="1" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D6" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1107,7 +1137,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1128,42 +1158,42 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>13</v>
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>14</v>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>15</v>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>